<commit_message>
Worked on binary search problem.
</commit_message>
<xml_diff>
--- a/Python-Scripts/Josephus_prb.xlsx
+++ b/Python-Scripts/Josephus_prb.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\github\Python3\Python-Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18319F4A-A935-40CC-A3E1-807EAC92A0D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976D347F-2F65-44F4-9302-8D9A0D589B76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6570" xr2:uid="{C255598B-2E3E-4565-BAB2-683F9625FF46}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6570" activeTab="1" xr2:uid="{C255598B-2E3E-4565-BAB2-683F9625FF46}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>a</t>
   </si>
@@ -126,18 +127,101 @@
   </si>
   <si>
     <t>= Step 6 - Step 5</t>
+  </si>
+  <si>
+    <t>e =</t>
+  </si>
+  <si>
+    <t>x =</t>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>= B * sqrt(x^3)</t>
+  </si>
+  <si>
+    <t>= -C * exp(-x/50)</t>
+  </si>
+  <si>
+    <t>= -D</t>
+  </si>
+  <si>
+    <t>= Step 6 + Step 7</t>
+  </si>
+  <si>
+    <t>= Step 5 - Step 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A </t>
+  </si>
+  <si>
+    <t>* x^(3/2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="169" formatCode="0.00000"/>
-    <numFmt numFmtId="171" formatCode="0.0000000"/>
-    <numFmt numFmtId="174" formatCode="0.0000000000"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000"/>
+    <numFmt numFmtId="172" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +255,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,96 +419,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -425,13 +514,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -748,9 +855,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE5D1BD-EE16-4E57-92DD-3C6102D97548}">
-  <dimension ref="A1:AH42"/>
+  <dimension ref="A1:AH62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
+    <sheetView topLeftCell="E19" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -763,13 +870,13 @@
     <col min="8" max="8" width="12.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="14.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" style="1" customWidth="1"/>
     <col min="18" max="18" width="11.5703125" style="1" customWidth="1"/>
     <col min="19" max="36" width="4" style="1" customWidth="1"/>
     <col min="37" max="16384" width="9.140625" style="1"/>
@@ -2100,6 +2207,12 @@
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="G29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="1">
+        <v>2.71828</v>
+      </c>
       <c r="J29" s="1" t="s">
         <v>6</v>
       </c>
@@ -2127,59 +2240,59 @@
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="J30" s="1">
-        <v>0.59912051</v>
+        <v>15.68387514</v>
       </c>
       <c r="K30" s="1">
         <f>H31</f>
-        <v>73.5</v>
+        <v>41.899174957954997</v>
       </c>
       <c r="L30" s="1">
-        <v>0.64030348000000004</v>
+        <v>1.2622228</v>
       </c>
       <c r="M30" s="1">
         <f>SQRT(H31^3)</f>
-        <v>630.13123633097257</v>
+        <v>271.21156636354732</v>
       </c>
       <c r="N30" s="1">
-        <v>-263.33721366999998</v>
+        <v>-695.23706505999996</v>
       </c>
       <c r="O30" s="1">
         <f>EXP(-H31/50)</f>
-        <v>0.22992548518672384</v>
+        <v>0.43258194637986919</v>
       </c>
       <c r="P30" s="1">
-        <v>-387.92069616999999</v>
+        <v>-698.72384731</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="E31" s="1">
         <v>1</v>
       </c>
-      <c r="H31" s="30">
-        <v>73.5</v>
+      <c r="H31" s="29">
+        <v>41.899174957954997</v>
       </c>
       <c r="K31" s="1">
         <f>J30*K30</f>
-        <v>44.035357484999999</v>
+        <v>657.14142850958092</v>
       </c>
       <c r="L31" s="26"/>
       <c r="M31" s="1">
         <f>M30*L30</f>
-        <v>403.47522347942419</v>
+        <v>342.32942268778248</v>
       </c>
       <c r="N31" s="26"/>
       <c r="O31" s="1">
         <f>N30*EXP(H31/50)</f>
-        <v>-1145.3154636431116</v>
+        <v>-1607.1800288435566</v>
       </c>
       <c r="P31" s="26"/>
       <c r="Q31" s="1">
         <f>P30</f>
-        <v>-387.92069616999999</v>
-      </c>
-      <c r="R31" s="29">
+        <v>-698.72384731</v>
+      </c>
+      <c r="R31" s="28">
         <f>SUM(K31:Q31)</f>
-        <v>-1085.7255788486873</v>
+        <v>-1306.4330249561931</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
@@ -2187,126 +2300,1079 @@
         <f>E31-128</f>
         <v>-127</v>
       </c>
-    </row>
-    <row r="33" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H32" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K33" s="31" t="s">
+      <c r="K33" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="L33" s="33">
+      <c r="L33" s="32">
         <f>SQRT(H31^3)</f>
-        <v>630.13123633097257</v>
+        <v>271.21156636354732</v>
       </c>
       <c r="N33" s="26"/>
       <c r="Q33" s="26"/>
     </row>
-    <row r="34" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J34" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K34" s="31" t="s">
+      <c r="K34" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="L34" s="34">
+      <c r="L34" s="33">
         <f>EXP(-H31/50)</f>
-        <v>0.22992548518672384</v>
-      </c>
-    </row>
-    <row r="35" spans="8:17" x14ac:dyDescent="0.25">
+        <v>0.43258194637986919</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K35" s="31" t="s">
+      <c r="K35" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="L35" s="34">
+      <c r="L35" s="33">
         <f>J30*H31</f>
-        <v>44.035357484999999</v>
-      </c>
-      <c r="M35" s="28"/>
+        <v>657.14142850958092</v>
+      </c>
+      <c r="M35" s="27"/>
       <c r="N35" s="26"/>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
-      <c r="Q35" s="28"/>
-    </row>
-    <row r="36" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="O35" s="35"/>
+      <c r="P35" s="35"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H36" s="1">
         <v>73.595368554161993</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K36" s="31" t="s">
+      <c r="K36" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="L36" s="34">
+      <c r="L36" s="33">
         <f>L30*M30</f>
-        <v>403.47522347942419</v>
-      </c>
-    </row>
-    <row r="37" spans="8:17" x14ac:dyDescent="0.25">
+        <v>342.32942268778248</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H37" s="1">
+        <v>41.899174957954997</v>
+      </c>
       <c r="J37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K37" s="31" t="s">
+      <c r="K37" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="L37" s="34">
+      <c r="L37" s="33">
         <f>N30*L34</f>
-        <v>-60.547936620794715</v>
-      </c>
-    </row>
-    <row r="38" spans="8:17" x14ac:dyDescent="0.25">
+        <v>-300.74700279908251</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J38" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K38" s="31" t="s">
+      <c r="K38" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="L38" s="33">
+      <c r="L38" s="32">
         <f>L35+L36</f>
-        <v>447.51058096442421</v>
-      </c>
-    </row>
-    <row r="39" spans="8:17" x14ac:dyDescent="0.25">
+        <v>999.47085119736334</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J39" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K39" s="31" t="s">
+      <c r="K39" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="L39" s="34">
+      <c r="L39" s="33">
         <f>L38+L37</f>
-        <v>386.96264434362951</v>
-      </c>
-    </row>
-    <row r="40" spans="8:17" x14ac:dyDescent="0.25">
+        <v>698.72384839828078</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J40" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K40" s="31" t="s">
+      <c r="K40" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="L40" s="35">
+      <c r="L40" s="34">
         <f>L39+P30</f>
-        <v>-0.95805182637047892</v>
-      </c>
-    </row>
-    <row r="41" spans="8:17" x14ac:dyDescent="0.25">
+        <v>1.0882807828238583E-6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J41" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K41" s="32"/>
-      <c r="L41" s="34"/>
-    </row>
-    <row r="42" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="K41" s="31"/>
+      <c r="L41" s="33"/>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H42" s="1">
+        <f>H29*H31</f>
+        <v>113.89368930470991</v>
+      </c>
       <c r="J42" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K42" s="32"/>
-      <c r="L42" s="34"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="33"/>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+      <c r="O49"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+      <c r="O52"/>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="N53"/>
+      <c r="O53"/>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+      <c r="O54"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="O55"/>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+      <c r="N56"/>
+      <c r="O56"/>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="N57"/>
+      <c r="O57"/>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B58"/>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="N58"/>
+      <c r="O58"/>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B59"/>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="O59"/>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60"/>
+      <c r="G60"/>
+      <c r="H60"/>
+      <c r="I60"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="N60"/>
+      <c r="O60"/>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+      <c r="N61"/>
+      <c r="O61"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62"/>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62"/>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62"/>
+      <c r="M62"/>
+      <c r="N62"/>
+      <c r="O62"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC199F2-F558-4B67-B3F5-BCEC1DBBC92C}">
+  <dimension ref="B1:P34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="4" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" style="1" customWidth="1"/>
+    <col min="17" max="34" width="4" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2.71828</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H2" s="38">
+        <v>0.59912051</v>
+      </c>
+      <c r="I2" s="1">
+        <f>F3</f>
+        <v>73.595368554161993</v>
+      </c>
+      <c r="J2" s="38">
+        <v>0.64030348000000004</v>
+      </c>
+      <c r="K2" s="1">
+        <f>SQRT(F3^3)</f>
+        <v>631.35805662522819</v>
+      </c>
+      <c r="L2" s="38">
+        <v>263.33721366999998</v>
+      </c>
+      <c r="M2" s="1">
+        <f>EXP(-F3/50)</f>
+        <v>0.22948734994105821</v>
+      </c>
+      <c r="N2" s="38">
+        <v>387.92069616999999</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E3" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="29">
+        <v>73.595368554161993</v>
+      </c>
+      <c r="I3" s="1">
+        <f>H2*I2</f>
+        <v>44.092494741807492</v>
+      </c>
+      <c r="J3" s="26"/>
+      <c r="K3" s="1">
+        <f>K2*J2</f>
+        <v>404.26076078317067</v>
+      </c>
+      <c r="L3" s="26"/>
+      <c r="M3" s="1">
+        <f>L2*EXP(F3/50)</f>
+        <v>1147.5020899306032</v>
+      </c>
+      <c r="N3" s="26"/>
+      <c r="O3" s="1">
+        <f>N2</f>
+        <v>387.92069616999999</v>
+      </c>
+      <c r="P3" s="28">
+        <f>SUM(I3:O3)</f>
+        <v>1983.7760416255812</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="32">
+        <f>SQRT(F3^3)</f>
+        <v>631.35805662522819</v>
+      </c>
+      <c r="L5" s="26"/>
+      <c r="O5" s="26"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="33">
+        <f>EXP(-F3/50)</f>
+        <v>0.22948734994105821</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="33">
+        <f>H2*F3</f>
+        <v>44.092494741807492</v>
+      </c>
+      <c r="K7" s="27"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+    </row>
+    <row r="8" spans="2:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="E8" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="1">
+        <v>73.595368554161993</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="33">
+        <f>J2*K2</f>
+        <v>404.26076078317067</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="E9" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1">
+        <v>41.899174957954997</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="32">
+        <f>J7+J8</f>
+        <v>448.35325552497818</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="33">
+        <f>-L2*M2</f>
+        <v>-60.432559305990502</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="37">
+        <f>-N2</f>
+        <v>-387.92069616999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="38">
+        <f>(-L2*M2)-N2</f>
+        <v>-448.35325547599047</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="33">
+        <f>J9+J12</f>
+        <v>4.8987715217663208E-8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I14" s="31"/>
+      <c r="J14" s="33"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L15" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15" s="41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16" s="42">
+        <f>H2</f>
+        <v>0.59912051</v>
+      </c>
+      <c r="I16" s="42">
+        <f>I2</f>
+        <v>73.595368554161993</v>
+      </c>
+      <c r="J16" s="42">
+        <f>J2</f>
+        <v>0.64030348000000004</v>
+      </c>
+      <c r="K16" s="42">
+        <f>K2</f>
+        <v>631.35805662522819</v>
+      </c>
+      <c r="L16" s="42">
+        <f>-L2</f>
+        <v>-263.33721366999998</v>
+      </c>
+      <c r="M16" s="42">
+        <f>M2</f>
+        <v>0.22948734994105821</v>
+      </c>
+      <c r="N16" s="42">
+        <f>-N2</f>
+        <v>-387.92069616999999</v>
+      </c>
+      <c r="O16" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17" s="42">
+        <f>H16*I16</f>
+        <v>44.092494741807492</v>
+      </c>
+      <c r="I17" s="42">
+        <f>J16*K16</f>
+        <v>404.26076078317067</v>
+      </c>
+      <c r="J17" s="42">
+        <f>L16*M16</f>
+        <v>-60.432559305990502</v>
+      </c>
+      <c r="K17" s="42">
+        <f>N16</f>
+        <v>-387.92069616999999</v>
+      </c>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18" s="42">
+        <f>H17+I17</f>
+        <v>448.35325552497818</v>
+      </c>
+      <c r="I18" s="42">
+        <f>J17+K17</f>
+        <v>-448.35325547599047</v>
+      </c>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19" s="42">
+        <f>H18+I18</f>
+        <v>4.8987715217663208E-8</v>
+      </c>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="42"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22" s="40">
+        <v>0.59912051</v>
+      </c>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40">
+        <v>0.64030348000000004</v>
+      </c>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40">
+        <v>263.33721366999998</v>
+      </c>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40">
+        <v>387.92069616999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23" s="40">
+        <v>15.68387514</v>
+      </c>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40">
+        <v>1.2622228</v>
+      </c>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40">
+        <v>695.23706505999996</v>
+      </c>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40">
+        <v>698.72384731</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tried to complete bin search problem.
</commit_message>
<xml_diff>
--- a/Python-Scripts/Josephus_prb.xlsx
+++ b/Python-Scripts/Josephus_prb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Python3\Python-Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\github\Python3\Python-Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AC327B-559C-4A2C-8D79-FF10BDA9A97C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F56293-3147-45BF-919B-02461518369F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12960" yWindow="270" windowWidth="15600" windowHeight="14475" activeTab="1" xr2:uid="{C255598B-2E3E-4565-BAB2-683F9625FF46}"/>
   </bookViews>
@@ -24,7 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="90">
   <si>
     <t>a</t>
   </si>
@@ -239,6 +238,547 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> - C/50x</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ax + Bx</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - C/50x*(ln e)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ax + Bx</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - C/50x*(1)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">X = </t>
+  </si>
+  <si>
+    <r>
+      <t>X(A + B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>√1 -C*0.02)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(A + B*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>√1 - C/0.02)</t>
+    </r>
+  </si>
+  <si>
+    <t>D/X</t>
+  </si>
+  <si>
+    <r>
+      <t>(A + B*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>√1 - C/0.02)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/D</t>
+    </r>
+  </si>
+  <si>
+    <t>1/x</t>
+  </si>
+  <si>
+    <r>
+      <t>5x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 40</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2/3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 8</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2/3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x = 8</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2/3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>√8</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">x = </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>√64</t>
+    </r>
+  </si>
+  <si>
+    <t>x = 4</t>
+  </si>
+  <si>
+    <r>
+      <t>x(5)(1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) = 40</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-x/50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.923116346386636</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>log</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0.923116346386636 = -x/50</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1/50e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.923116346386636</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 0.923116346386636*(50)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ce</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-x/50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>263.33721367*e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-x/50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-x/50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = 0/263.33721367</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ax + Bx</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> - Ce</t>
     </r>
     <r>
@@ -250,12 +790,83 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">-x/50 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- D</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">= </t>
+  </si>
+  <si>
+    <t>D - Ax</t>
+  </si>
+  <si>
+    <r>
+      <t>Bx</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Ce</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>-x/50</t>
     </r>
   </si>
   <si>
-    <r>
-      <t>Ax + Bx</t>
+    <t xml:space="preserve">D = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B = </t>
+  </si>
+  <si>
+    <t>D - A =</t>
+  </si>
+  <si>
+    <t>387.32157566x</t>
+  </si>
+  <si>
+    <r>
+      <t>(0.64030348 * x</t>
     </r>
     <r>
       <rPr>
@@ -266,6 +877,49 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>1/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>0.4099885465001104x</t>
+  </si>
+  <si>
+    <t>698.72384731 - 15.68387514x</t>
+  </si>
+  <si>
+    <r>
+      <t>1.2622228X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>3/2</t>
     </r>
     <r>
@@ -276,12 +930,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - C/50x</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Ax + Bx</t>
+      <t xml:space="preserve"> - 695.23706506*e</t>
     </r>
     <r>
       <rPr>
@@ -292,6 +941,48 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>-x/50</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.2622228 * x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - 5.2667442734</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.2622228 * x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>3/2</t>
     </r>
     <r>
@@ -302,12 +993,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - C/50x*(ln e)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Ax + Bx</t>
+      <t xml:space="preserve"> - 695.23706506 * xLNe</t>
     </r>
     <r>
       <rPr>
@@ -318,6 +1004,48 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>1/50</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.2622228 * x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - 695.23706506 * Lne(1/50)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>15.68387514X + 1.2622228X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>3/2</t>
     </r>
     <r>
@@ -328,69 +1056,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - C/50x*(1)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">X = </t>
-  </si>
-  <si>
-    <r>
-      <t>X(A + B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>√1 -C*0.02)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>(A + B*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>√1 - C/0.02)</t>
-    </r>
-  </si>
-  <si>
-    <t>D/X</t>
-  </si>
-  <si>
-    <r>
-      <t>(A + B*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>√1 - C/0.02)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/D</t>
-    </r>
-  </si>
-  <si>
-    <t>1/x</t>
+      <t xml:space="preserve"> - 695.23706506*e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-x/50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - 698.72384731 = 3.423575463220118</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -403,7 +1091,7 @@
     <numFmt numFmtId="166" formatCode="0.0000000000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,6 +1146,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -615,7 +1310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -738,6 +1433,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2955,10 +3659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC199F2-F558-4B67-B3F5-BCEC1DBBC92C}">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2967,7 +3671,7 @@
     <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" customWidth="1"/>
@@ -3232,31 +3936,31 @@
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16" s="42">
-        <f>D2</f>
+        <f t="shared" ref="D16:J16" si="0">D2</f>
         <v>0.59912051</v>
       </c>
       <c r="E16" s="42">
-        <f>E2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F16" s="42">
-        <f>F2</f>
+        <f t="shared" si="0"/>
         <v>0.64030348000000004</v>
       </c>
       <c r="G16" s="42">
-        <f>G2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H16" s="42">
-        <f>H2</f>
+        <f t="shared" si="0"/>
         <v>263.33721366999998</v>
       </c>
       <c r="I16" s="42">
-        <f>I2</f>
+        <f t="shared" si="0"/>
         <v>0.92311634638663576</v>
       </c>
       <c r="J16" s="42">
-        <f>J2</f>
+        <f t="shared" si="0"/>
         <v>387.92069616999999</v>
       </c>
       <c r="K16" s="42">
@@ -3462,25 +4166,33 @@
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
+      <c r="H29" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="I29" s="1">
+        <v>15.68387514</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
-      <c r="E30" t="s">
-        <v>49</v>
+      <c r="E30" s="37" t="s">
+        <v>72</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G30" t="s">
-        <v>48</v>
-      </c>
-      <c r="H30"/>
-      <c r="I30"/>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1.2622228</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A31"/>
@@ -3488,7 +4200,7 @@
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>47</v>
@@ -3496,8 +4208,12 @@
       <c r="G31" t="s">
         <v>48</v>
       </c>
-      <c r="H31"/>
-      <c r="I31"/>
+      <c r="H31" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="I31" s="1">
+        <v>695.23706505999996</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A32"/>
@@ -3505,7 +4221,7 @@
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>47</v>
@@ -3513,8 +4229,12 @@
       <c r="G32" t="s">
         <v>48</v>
       </c>
-      <c r="H32"/>
-      <c r="I32"/>
+      <c r="H32" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I32" s="1">
+        <v>698.72384731</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A33"/>
@@ -3522,7 +4242,7 @@
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>47</v>
@@ -3539,7 +4259,7 @@
       <c r="C34"/>
       <c r="D34" s="26"/>
       <c r="E34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>47</v>
@@ -3547,34 +4267,36 @@
       <c r="G34" t="s">
         <v>48</v>
       </c>
-      <c r="H34"/>
+      <c r="H34" s="37" t="s">
+        <v>80</v>
+      </c>
       <c r="I34"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D39" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E39" s="1">
         <f>1/((D22+F22*SQRT(1)-H22*B1*0.02)/J22)</f>
@@ -3584,10 +4306,199 @@
         <v>47</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E41" s="30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E43" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E44" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="F44" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G44" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="H44" s="46"/>
+    </row>
+    <row r="45" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E45" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E46" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="F46" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G46" s="1">
+        <v>387.32157566000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E47" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G47" s="1">
+        <v>387.32157566000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E48" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="F48" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G48" s="1">
+        <f>(387.32157566+5.2667442734)^2</f>
+        <v>154125.58894812962</v>
+      </c>
+    </row>
+    <row r="49" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E49" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="F49" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G49" s="1">
+        <f>(387.32157566+5.2667442734)^2</f>
+        <v>154125.58894812962</v>
+      </c>
+    </row>
+    <row r="50" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E50" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G52" s="1">
+        <v>154125.58894813</v>
+      </c>
+    </row>
+    <row r="57" spans="5:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E57" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="H57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="5:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="5:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E59" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="5:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E60" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H60" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="5:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E61" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H61" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="I61" s="1">
+        <f>I34*50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H62" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="I62" s="1">
+        <f>LN(46.1558173193318)</f>
+        <v>3.8320230054281463</v>
+      </c>
+    </row>
+    <row r="64" spans="5:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E64" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H64" s="1">
+        <f>1/50*B1</f>
+        <v>5.43656E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="5:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="E65" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="5:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="5:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="H67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="5:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E71" s="1">
+        <f>(3*89*677*947)/(2^7 * 5^8)</f>
+        <v>3.4235754599999999</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G44:H44"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>